<commit_message>
Fixed problem with path
</commit_message>
<xml_diff>
--- a/src/excel/plan_full_new_multiple_correct.xlsx
+++ b/src/excel/plan_full_new_multiple_correct.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shchelik.gs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gshch\Code\projects\study_plan_test\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3EBF20-B5E1-43D8-B2E5-BF62A58D157C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5895" tabRatio="212"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="212" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Предметы" sheetId="1" r:id="rId1"/>
     <sheet name="Планы" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" refMode="R1C1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="363">
   <si>
     <t>Код</t>
   </si>
@@ -1114,7 +1115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1366,6 +1367,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1401,6 +1419,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1576,45 +1611,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:AA187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+    <sheetView topLeftCell="A160" workbookViewId="0">
       <selection activeCell="J170" sqref="J170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="11.5" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="36.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" style="1" customWidth="1"/>
     <col min="19" max="19" width="10" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.6640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="20.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.83203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="16.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.77734375" style="1" customWidth="1"/>
     <col min="24" max="24" width="10" style="1" customWidth="1"/>
     <col min="25" max="25" width="13.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.44140625" style="1" customWidth="1"/>
     <col min="27" max="27" width="21.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1701,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>17916</v>
       </c>
@@ -1770,7 +1805,7 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>17916</v>
       </c>
@@ -1839,7 +1874,7 @@
       <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
     </row>
-    <row r="4" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>17916</v>
       </c>
@@ -1906,7 +1941,7 @@
       </c>
       <c r="AA4" s="12"/>
     </row>
-    <row r="5" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>17916</v>
       </c>
@@ -1973,7 +2008,7 @@
       </c>
       <c r="AA5" s="12"/>
     </row>
-    <row r="6" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>17916</v>
       </c>
@@ -2040,7 +2075,7 @@
       </c>
       <c r="AA6" s="12"/>
     </row>
-    <row r="7" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>17916</v>
       </c>
@@ -2107,7 +2142,7 @@
       </c>
       <c r="AA7" s="12"/>
     </row>
-    <row r="8" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>17916</v>
       </c>
@@ -2174,7 +2209,7 @@
       </c>
       <c r="AA8" s="12"/>
     </row>
-    <row r="9" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>17916</v>
       </c>
@@ -2241,7 +2276,7 @@
       </c>
       <c r="AA9" s="12"/>
     </row>
-    <row r="10" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>17916</v>
       </c>
@@ -2308,7 +2343,7 @@
       </c>
       <c r="AA10" s="12"/>
     </row>
-    <row r="11" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>17916</v>
       </c>
@@ -2375,7 +2410,7 @@
       </c>
       <c r="AA11" s="12"/>
     </row>
-    <row r="12" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>17916</v>
       </c>
@@ -2444,7 +2479,7 @@
       </c>
       <c r="AA12" s="12"/>
     </row>
-    <row r="13" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>17916</v>
       </c>
@@ -2513,7 +2548,7 @@
       </c>
       <c r="AA13" s="12"/>
     </row>
-    <row r="14" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>17916</v>
       </c>
@@ -2582,7 +2617,7 @@
       </c>
       <c r="AA14" s="12"/>
     </row>
-    <row r="15" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>17916</v>
       </c>
@@ -2651,7 +2686,7 @@
       </c>
       <c r="AA15" s="12"/>
     </row>
-    <row r="16" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>17916</v>
       </c>
@@ -2720,7 +2755,7 @@
       </c>
       <c r="AA16" s="12"/>
     </row>
-    <row r="17" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>17916</v>
       </c>
@@ -2789,7 +2824,7 @@
       </c>
       <c r="AA17" s="12"/>
     </row>
-    <row r="18" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>17916</v>
       </c>
@@ -2858,7 +2893,7 @@
       </c>
       <c r="AA18" s="12"/>
     </row>
-    <row r="19" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>17916</v>
       </c>
@@ -2927,7 +2962,7 @@
       </c>
       <c r="AA19" s="12"/>
     </row>
-    <row r="20" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>17916</v>
       </c>
@@ -2996,7 +3031,7 @@
       </c>
       <c r="AA20" s="12"/>
     </row>
-    <row r="21" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>17916</v>
       </c>
@@ -3065,7 +3100,7 @@
       </c>
       <c r="AA21" s="12"/>
     </row>
-    <row r="22" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>17916</v>
       </c>
@@ -3134,7 +3169,7 @@
       </c>
       <c r="AA22" s="12"/>
     </row>
-    <row r="23" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>17916</v>
       </c>
@@ -3203,7 +3238,7 @@
       </c>
       <c r="AA23" s="12"/>
     </row>
-    <row r="24" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>17916</v>
       </c>
@@ -3272,7 +3307,7 @@
       </c>
       <c r="AA24" s="12"/>
     </row>
-    <row r="25" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>17916</v>
       </c>
@@ -3341,7 +3376,7 @@
       </c>
       <c r="AA25" s="12"/>
     </row>
-    <row r="26" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>17916</v>
       </c>
@@ -3410,7 +3445,7 @@
       </c>
       <c r="AA26" s="12"/>
     </row>
-    <row r="27" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>17916</v>
       </c>
@@ -3479,7 +3514,7 @@
       </c>
       <c r="AA27" s="12"/>
     </row>
-    <row r="28" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>17916</v>
       </c>
@@ -3546,7 +3581,7 @@
       </c>
       <c r="AA28" s="12"/>
     </row>
-    <row r="29" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>17916</v>
       </c>
@@ -3613,7 +3648,7 @@
       </c>
       <c r="AA29" s="12"/>
     </row>
-    <row r="30" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>17916</v>
       </c>
@@ -3680,7 +3715,7 @@
       </c>
       <c r="AA30" s="12"/>
     </row>
-    <row r="31" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>17916</v>
       </c>
@@ -3747,7 +3782,7 @@
       </c>
       <c r="AA31" s="12"/>
     </row>
-    <row r="32" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>17916</v>
       </c>
@@ -3814,7 +3849,7 @@
       </c>
       <c r="AA32" s="12"/>
     </row>
-    <row r="33" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>17916</v>
       </c>
@@ -3881,7 +3916,7 @@
       </c>
       <c r="AA33" s="12"/>
     </row>
-    <row r="34" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>17916</v>
       </c>
@@ -3948,7 +3983,7 @@
       </c>
       <c r="AA34" s="12"/>
     </row>
-    <row r="35" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>17916</v>
       </c>
@@ -4015,7 +4050,7 @@
       </c>
       <c r="AA35" s="12"/>
     </row>
-    <row r="36" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>17916</v>
       </c>
@@ -4084,7 +4119,7 @@
       </c>
       <c r="AA36" s="12"/>
     </row>
-    <row r="37" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>17916</v>
       </c>
@@ -4153,7 +4188,7 @@
       </c>
       <c r="AA37" s="12"/>
     </row>
-    <row r="38" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>17916</v>
       </c>
@@ -4222,7 +4257,7 @@
       </c>
       <c r="AA38" s="12"/>
     </row>
-    <row r="39" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>17916</v>
       </c>
@@ -4291,7 +4326,7 @@
       </c>
       <c r="AA39" s="12"/>
     </row>
-    <row r="40" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>17916</v>
       </c>
@@ -4360,7 +4395,7 @@
       </c>
       <c r="AA40" s="12"/>
     </row>
-    <row r="41" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>17916</v>
       </c>
@@ -4429,7 +4464,7 @@
       </c>
       <c r="AA41" s="12"/>
     </row>
-    <row r="42" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>17916</v>
       </c>
@@ -4498,7 +4533,7 @@
       </c>
       <c r="AA42" s="12"/>
     </row>
-    <row r="43" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>17916</v>
       </c>
@@ -4567,7 +4602,7 @@
       </c>
       <c r="AA43" s="12"/>
     </row>
-    <row r="44" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>17916</v>
       </c>
@@ -4640,7 +4675,7 @@
       </c>
       <c r="AA44" s="12"/>
     </row>
-    <row r="45" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>17916</v>
       </c>
@@ -4713,7 +4748,7 @@
       </c>
       <c r="AA45" s="12"/>
     </row>
-    <row r="46" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>17916</v>
       </c>
@@ -4786,7 +4821,7 @@
       </c>
       <c r="AA46" s="12"/>
     </row>
-    <row r="47" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>17916</v>
       </c>
@@ -4859,7 +4894,7 @@
       </c>
       <c r="AA47" s="12"/>
     </row>
-    <row r="48" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>17916</v>
       </c>
@@ -4932,7 +4967,7 @@
       </c>
       <c r="AA48" s="12"/>
     </row>
-    <row r="49" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>17916</v>
       </c>
@@ -5005,7 +5040,7 @@
       </c>
       <c r="AA49" s="12"/>
     </row>
-    <row r="50" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>17916</v>
       </c>
@@ -5078,7 +5113,7 @@
       </c>
       <c r="AA50" s="12"/>
     </row>
-    <row r="51" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>17916</v>
       </c>
@@ -5151,7 +5186,7 @@
       </c>
       <c r="AA51" s="12"/>
     </row>
-    <row r="52" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>17916</v>
       </c>
@@ -5224,7 +5259,7 @@
       </c>
       <c r="AA52" s="12"/>
     </row>
-    <row r="53" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>17916</v>
       </c>
@@ -5297,7 +5332,7 @@
       </c>
       <c r="AA53" s="12"/>
     </row>
-    <row r="54" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>17916</v>
       </c>
@@ -5370,7 +5405,7 @@
       </c>
       <c r="AA54" s="12"/>
     </row>
-    <row r="55" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>17916</v>
       </c>
@@ -5443,7 +5478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>17916</v>
       </c>
@@ -5516,7 +5551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>17916</v>
       </c>
@@ -5589,7 +5624,7 @@
       </c>
       <c r="AA57" s="12"/>
     </row>
-    <row r="58" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>17916</v>
       </c>
@@ -5662,7 +5697,7 @@
       </c>
       <c r="AA58" s="12"/>
     </row>
-    <row r="59" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>17916</v>
       </c>
@@ -5735,7 +5770,7 @@
       </c>
       <c r="AA59" s="12"/>
     </row>
-    <row r="60" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>17916</v>
       </c>
@@ -5808,7 +5843,7 @@
       </c>
       <c r="AA60" s="12"/>
     </row>
-    <row r="61" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>17916</v>
       </c>
@@ -5881,7 +5916,7 @@
       </c>
       <c r="AA61" s="12"/>
     </row>
-    <row r="62" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>17916</v>
       </c>
@@ -5954,7 +5989,7 @@
       </c>
       <c r="AA62" s="12"/>
     </row>
-    <row r="63" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>17916</v>
       </c>
@@ -6021,7 +6056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>17916</v>
       </c>
@@ -6088,7 +6123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>17916</v>
       </c>
@@ -6155,7 +6190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>17916</v>
       </c>
@@ -6222,7 +6257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>17916</v>
       </c>
@@ -6289,7 +6324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>17916</v>
       </c>
@@ -6362,7 +6397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>17916</v>
       </c>
@@ -6435,7 +6470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>17916</v>
       </c>
@@ -6508,7 +6543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>17916</v>
       </c>
@@ -6581,7 +6616,7 @@
       </c>
       <c r="AA71" s="12"/>
     </row>
-    <row r="72" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>17916</v>
       </c>
@@ -6654,7 +6689,7 @@
       </c>
       <c r="AA72" s="12"/>
     </row>
-    <row r="73" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>17916</v>
       </c>
@@ -6725,7 +6760,7 @@
       </c>
       <c r="AA73" s="12"/>
     </row>
-    <row r="74" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>17916</v>
       </c>
@@ -6798,7 +6833,7 @@
       </c>
       <c r="AA74" s="12"/>
     </row>
-    <row r="75" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>17916</v>
       </c>
@@ -6871,7 +6906,7 @@
       </c>
       <c r="AA75" s="12"/>
     </row>
-    <row r="76" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>17916</v>
       </c>
@@ -6944,7 +6979,7 @@
       </c>
       <c r="AA76" s="12"/>
     </row>
-    <row r="77" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>17916</v>
       </c>
@@ -7013,7 +7048,7 @@
       <c r="Z77" s="12"/>
       <c r="AA77" s="12"/>
     </row>
-    <row r="78" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>17916</v>
       </c>
@@ -7080,7 +7115,7 @@
       </c>
       <c r="AA78" s="12"/>
     </row>
-    <row r="79" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>17916</v>
       </c>
@@ -7145,7 +7180,7 @@
       </c>
       <c r="AA79" s="12"/>
     </row>
-    <row r="80" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>17916</v>
       </c>
@@ -7210,7 +7245,7 @@
       </c>
       <c r="AA80" s="12"/>
     </row>
-    <row r="81" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>17916</v>
       </c>
@@ -7275,7 +7310,7 @@
       </c>
       <c r="AA81" s="12"/>
     </row>
-    <row r="82" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>17916</v>
       </c>
@@ -7340,7 +7375,7 @@
       </c>
       <c r="AA82" s="12"/>
     </row>
-    <row r="83" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>17916</v>
       </c>
@@ -7405,7 +7440,7 @@
       </c>
       <c r="AA83" s="12"/>
     </row>
-    <row r="84" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>17916</v>
       </c>
@@ -7474,7 +7509,7 @@
       <c r="Z84" s="12"/>
       <c r="AA84" s="12"/>
     </row>
-    <row r="85" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>17916</v>
       </c>
@@ -7543,7 +7578,7 @@
       </c>
       <c r="AA85" s="12"/>
     </row>
-    <row r="86" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>17916</v>
       </c>
@@ -7612,7 +7647,7 @@
       </c>
       <c r="AA86" s="12"/>
     </row>
-    <row r="87" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>17916</v>
       </c>
@@ -7681,7 +7716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>17916</v>
       </c>
@@ -7750,7 +7785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>17916</v>
       </c>
@@ -7819,7 +7854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>17916</v>
       </c>
@@ -7888,7 +7923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>17916</v>
       </c>
@@ -7957,7 +7992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>17916</v>
       </c>
@@ -8026,7 +8061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>17916</v>
       </c>
@@ -8095,7 +8130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>17916</v>
       </c>
@@ -8162,7 +8197,7 @@
       <c r="Z94" s="12"/>
       <c r="AA94" s="12"/>
     </row>
-    <row r="95" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>17916</v>
       </c>
@@ -8231,7 +8266,7 @@
       <c r="Z95" s="12"/>
       <c r="AA95" s="12"/>
     </row>
-    <row r="96" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>17916</v>
       </c>
@@ -8300,7 +8335,7 @@
       <c r="Z96" s="12"/>
       <c r="AA96" s="12"/>
     </row>
-    <row r="97" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>17916</v>
       </c>
@@ -8369,7 +8404,7 @@
       <c r="Z97" s="12"/>
       <c r="AA97" s="12"/>
     </row>
-    <row r="98" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>17916</v>
       </c>
@@ -8438,7 +8473,7 @@
       <c r="Z98" s="12"/>
       <c r="AA98" s="12"/>
     </row>
-    <row r="99" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>17916</v>
       </c>
@@ -8507,7 +8542,7 @@
       <c r="Z99" s="12"/>
       <c r="AA99" s="12"/>
     </row>
-    <row r="100" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A100" s="8">
         <v>17916</v>
       </c>
@@ -8576,7 +8611,7 @@
       <c r="Z100" s="12"/>
       <c r="AA100" s="12"/>
     </row>
-    <row r="101" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <v>17916</v>
       </c>
@@ -8639,7 +8674,7 @@
       <c r="Z101" s="12"/>
       <c r="AA101" s="12"/>
     </row>
-    <row r="102" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A102" s="8">
         <v>17916</v>
       </c>
@@ -8702,7 +8737,7 @@
       <c r="Z102" s="12"/>
       <c r="AA102" s="12"/>
     </row>
-    <row r="103" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A103" s="8">
         <v>17916</v>
       </c>
@@ -8765,7 +8800,7 @@
       <c r="Z103" s="12"/>
       <c r="AA103" s="12"/>
     </row>
-    <row r="104" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>17916</v>
       </c>
@@ -8828,7 +8863,7 @@
       <c r="Z104" s="12"/>
       <c r="AA104" s="12"/>
     </row>
-    <row r="105" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>17916</v>
       </c>
@@ -8889,7 +8924,7 @@
       <c r="Z105" s="12"/>
       <c r="AA105" s="12"/>
     </row>
-    <row r="106" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A106" s="8">
         <v>17916</v>
       </c>
@@ -8962,7 +8997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="8">
         <v>17916</v>
       </c>
@@ -9035,7 +9070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A108" s="8">
         <v>17916</v>
       </c>
@@ -9102,7 +9137,7 @@
       <c r="Z108" s="12"/>
       <c r="AA108" s="12"/>
     </row>
-    <row r="109" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A109" s="8">
         <v>17916</v>
       </c>
@@ -9169,7 +9204,7 @@
       <c r="Z109" s="12"/>
       <c r="AA109" s="12"/>
     </row>
-    <row r="110" spans="1:27" ht="11.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" ht="11.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A110" s="8">
         <v>17916</v>
       </c>
@@ -9238,7 +9273,7 @@
       <c r="Z110" s="12"/>
       <c r="AA110" s="12"/>
     </row>
-    <row r="111" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A111" s="8">
         <v>17921</v>
       </c>
@@ -9305,7 +9340,7 @@
       <c r="Z111" s="12"/>
       <c r="AA111" s="12"/>
     </row>
-    <row r="112" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A112" s="8">
         <v>17921</v>
       </c>
@@ -9372,7 +9407,7 @@
       <c r="Z112" s="12"/>
       <c r="AA112" s="12"/>
     </row>
-    <row r="113" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A113" s="8">
         <v>17921</v>
       </c>
@@ -9437,7 +9472,7 @@
       <c r="Z113" s="12"/>
       <c r="AA113" s="12"/>
     </row>
-    <row r="114" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A114" s="8">
         <v>17921</v>
       </c>
@@ -9506,7 +9541,7 @@
       </c>
       <c r="AA114" s="12"/>
     </row>
-    <row r="115" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A115" s="8">
         <v>17921</v>
       </c>
@@ -9571,7 +9606,7 @@
       <c r="Z115" s="12"/>
       <c r="AA115" s="12"/>
     </row>
-    <row r="116" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A116" s="8">
         <v>17921</v>
       </c>
@@ -9636,7 +9671,7 @@
       <c r="Z116" s="12"/>
       <c r="AA116" s="12"/>
     </row>
-    <row r="117" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A117" s="8">
         <v>17921</v>
       </c>
@@ -9703,7 +9738,7 @@
       <c r="Z117" s="12"/>
       <c r="AA117" s="12"/>
     </row>
-    <row r="118" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <v>17921</v>
       </c>
@@ -9770,7 +9805,7 @@
       <c r="Z118" s="12"/>
       <c r="AA118" s="12"/>
     </row>
-    <row r="119" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A119" s="8">
         <v>17921</v>
       </c>
@@ -9837,7 +9872,7 @@
       <c r="Z119" s="12"/>
       <c r="AA119" s="12"/>
     </row>
-    <row r="120" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A120" s="8">
         <v>17921</v>
       </c>
@@ -9904,7 +9939,7 @@
       <c r="Z120" s="12"/>
       <c r="AA120" s="12"/>
     </row>
-    <row r="121" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A121" s="8">
         <v>17921</v>
       </c>
@@ -9971,7 +10006,7 @@
       </c>
       <c r="AA121" s="12"/>
     </row>
-    <row r="122" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <v>17921</v>
       </c>
@@ -10036,7 +10071,7 @@
       </c>
       <c r="AA122" s="12"/>
     </row>
-    <row r="123" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A123" s="8">
         <v>17921</v>
       </c>
@@ -10101,7 +10136,7 @@
       </c>
       <c r="AA123" s="12"/>
     </row>
-    <row r="124" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="8">
         <v>17921</v>
       </c>
@@ -10166,7 +10201,7 @@
       <c r="Z124" s="12"/>
       <c r="AA124" s="12"/>
     </row>
-    <row r="125" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A125" s="8">
         <v>17921</v>
       </c>
@@ -10227,7 +10262,7 @@
       <c r="Z125" s="12"/>
       <c r="AA125" s="12"/>
     </row>
-    <row r="126" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A126" s="8">
         <v>17921</v>
       </c>
@@ -10298,7 +10333,7 @@
       </c>
       <c r="AA126" s="12"/>
     </row>
-    <row r="127" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A127" s="8">
         <v>17921</v>
       </c>
@@ -10369,7 +10404,7 @@
       </c>
       <c r="AA127" s="12"/>
     </row>
-    <row r="128" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A128" s="8">
         <v>17921</v>
       </c>
@@ -10434,7 +10469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A129" s="8">
         <v>17921</v>
       </c>
@@ -10499,7 +10534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A130" s="8">
         <v>17921</v>
       </c>
@@ -10564,7 +10599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A131" s="8">
         <v>17921</v>
       </c>
@@ -10629,7 +10664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A132" s="8">
         <v>17921</v>
       </c>
@@ -10700,7 +10735,7 @@
       </c>
       <c r="AA132" s="12"/>
     </row>
-    <row r="133" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A133" s="8">
         <v>17921</v>
       </c>
@@ -10771,7 +10806,7 @@
       </c>
       <c r="AA133" s="12"/>
     </row>
-    <row r="134" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A134" s="8">
         <v>17921</v>
       </c>
@@ -10846,7 +10881,7 @@
       </c>
       <c r="AA134" s="12"/>
     </row>
-    <row r="135" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A135" s="8">
         <v>17921</v>
       </c>
@@ -10921,7 +10956,7 @@
       </c>
       <c r="AA135" s="12"/>
     </row>
-    <row r="136" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A136" s="8">
         <v>17921</v>
       </c>
@@ -10996,7 +11031,7 @@
       </c>
       <c r="AA136" s="12"/>
     </row>
-    <row r="137" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A137" s="8">
         <v>17921</v>
       </c>
@@ -11071,7 +11106,7 @@
       </c>
       <c r="AA137" s="12"/>
     </row>
-    <row r="138" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A138" s="8">
         <v>17922</v>
       </c>
@@ -11142,7 +11177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A139" s="8">
         <v>17922</v>
       </c>
@@ -11213,7 +11248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A140" s="8">
         <v>17922</v>
       </c>
@@ -11278,7 +11313,7 @@
       <c r="Z140" s="12"/>
       <c r="AA140" s="12"/>
     </row>
-    <row r="141" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="8">
         <v>17922</v>
       </c>
@@ -11347,7 +11382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A142" s="8">
         <v>17922</v>
       </c>
@@ -11412,7 +11447,7 @@
       <c r="Z142" s="12"/>
       <c r="AA142" s="12"/>
     </row>
-    <row r="143" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A143" s="8">
         <v>17922</v>
       </c>
@@ -11485,7 +11520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A144" s="8">
         <v>17922</v>
       </c>
@@ -11556,7 +11591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A145" s="8">
         <v>17922</v>
       </c>
@@ -11627,7 +11662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A146" s="8">
         <v>17922</v>
       </c>
@@ -11696,7 +11731,7 @@
       </c>
       <c r="AA146" s="12"/>
     </row>
-    <row r="147" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A147" s="8">
         <v>17922</v>
       </c>
@@ -11765,7 +11800,7 @@
       </c>
       <c r="AA147" s="12"/>
     </row>
-    <row r="148" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A148" s="8">
         <v>17922</v>
       </c>
@@ -11830,7 +11865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A149" s="8">
         <v>17922</v>
       </c>
@@ -11891,7 +11926,7 @@
       <c r="Z149" s="12"/>
       <c r="AA149" s="12"/>
     </row>
-    <row r="150" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A150" s="8">
         <v>17922</v>
       </c>
@@ -11962,7 +11997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A151" s="8">
         <v>17922</v>
       </c>
@@ -12033,7 +12068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A152" s="8">
         <v>17922</v>
       </c>
@@ -12098,7 +12133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A153" s="8">
         <v>17922</v>
       </c>
@@ -12163,7 +12198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A154" s="8">
         <v>17922</v>
       </c>
@@ -12234,7 +12269,7 @@
       </c>
       <c r="AA154" s="12"/>
     </row>
-    <row r="155" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A155" s="8">
         <v>17922</v>
       </c>
@@ -12305,7 +12340,7 @@
       </c>
       <c r="AA155" s="12"/>
     </row>
-    <row r="156" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A156" s="8">
         <v>17922</v>
       </c>
@@ -12380,7 +12415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A157" s="8">
         <v>17922</v>
       </c>
@@ -12455,7 +12490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="8">
         <v>17923</v>
       </c>
@@ -12522,7 +12557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A159" s="8">
         <v>17923</v>
       </c>
@@ -12589,7 +12624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A160" s="8">
         <v>17923</v>
       </c>
@@ -12660,7 +12695,7 @@
       </c>
       <c r="AA160" s="12"/>
     </row>
-    <row r="161" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A161" s="8">
         <v>17923</v>
       </c>
@@ -12729,7 +12764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A162" s="8">
         <v>17923</v>
       </c>
@@ -12796,7 +12831,7 @@
       <c r="Z162" s="12"/>
       <c r="AA162" s="12"/>
     </row>
-    <row r="163" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A163" s="8">
         <v>17923</v>
       </c>
@@ -12863,7 +12898,7 @@
       <c r="Z163" s="12"/>
       <c r="AA163" s="12"/>
     </row>
-    <row r="164" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A164" s="8">
         <v>17923</v>
       </c>
@@ -12932,7 +12967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A165" s="8">
         <v>17923</v>
       </c>
@@ -12997,7 +13032,7 @@
       <c r="Z165" s="12"/>
       <c r="AA165" s="12"/>
     </row>
-    <row r="166" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A166" s="8">
         <v>17923</v>
       </c>
@@ -13062,7 +13097,7 @@
       </c>
       <c r="AA166" s="12"/>
     </row>
-    <row r="167" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A167" s="8">
         <v>17923</v>
       </c>
@@ -13129,7 +13164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A168" s="8">
         <v>17923</v>
       </c>
@@ -13196,7 +13231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A169" s="8">
         <v>17923</v>
       </c>
@@ -13257,7 +13292,7 @@
       <c r="Z169" s="12"/>
       <c r="AA169" s="12"/>
     </row>
-    <row r="170" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A170" s="8">
         <v>17923</v>
       </c>
@@ -13324,7 +13359,7 @@
       <c r="Z170" s="12"/>
       <c r="AA170" s="12"/>
     </row>
-    <row r="171" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A171" s="8">
         <v>17923</v>
       </c>
@@ -13391,7 +13426,7 @@
       <c r="Z171" s="12"/>
       <c r="AA171" s="12"/>
     </row>
-    <row r="172" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A172" s="8">
         <v>17923</v>
       </c>
@@ -13458,7 +13493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A173" s="8">
         <v>17923</v>
       </c>
@@ -13525,7 +13560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A174" s="8">
         <v>17923</v>
       </c>
@@ -13590,7 +13625,7 @@
       </c>
       <c r="AA174" s="12"/>
     </row>
-    <row r="175" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="8">
         <v>17923</v>
       </c>
@@ -13661,7 +13696,7 @@
       </c>
       <c r="AA175" s="12"/>
     </row>
-    <row r="176" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A176" s="8">
         <v>17923</v>
       </c>
@@ -13732,7 +13767,7 @@
       </c>
       <c r="AA176" s="12"/>
     </row>
-    <row r="177" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A177" s="8">
         <v>17923</v>
       </c>
@@ -13803,7 +13838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A178" s="8">
         <v>17923</v>
       </c>
@@ -13878,7 +13913,7 @@
       </c>
       <c r="AA178" s="12"/>
     </row>
-    <row r="179" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A179" s="8">
         <v>17923</v>
       </c>
@@ -13953,7 +13988,7 @@
       </c>
       <c r="AA179" s="12"/>
     </row>
-    <row r="180" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A180" s="8">
         <v>17923</v>
       </c>
@@ -14028,7 +14063,7 @@
       </c>
       <c r="AA180" s="12"/>
     </row>
-    <row r="181" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A181" s="8">
         <v>17923</v>
       </c>
@@ -14103,7 +14138,7 @@
       </c>
       <c r="AA181" s="12"/>
     </row>
-    <row r="182" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A182" s="8">
         <v>17923</v>
       </c>
@@ -14172,7 +14207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A183" s="8">
         <v>17923</v>
       </c>
@@ -14241,7 +14276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A184" s="8">
         <v>17923</v>
       </c>
@@ -14310,7 +14345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A185" s="8">
         <v>17923</v>
       </c>
@@ -14379,7 +14414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A186" s="8">
         <v>17923</v>
       </c>
@@ -14448,7 +14483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:27" ht="21.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:27" ht="22" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A187" s="8">
         <v>17923</v>
       </c>
@@ -14524,21 +14559,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="89.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="15" customFormat="1" ht="12.5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -14548,43 +14584,45 @@
       <c r="C1" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>2</v>
+      <c r="D1" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -14604,8 +14642,9 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
-    </row>
-    <row r="2" spans="1:35" s="15" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ1" s="1"/>
+    </row>
+    <row r="2" spans="1:36" s="15" customFormat="1" ht="11.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>17916</v>
       </c>
@@ -14613,43 +14652,43 @@
         <v>14</v>
       </c>
       <c r="C2" s="16"/>
-      <c r="D2" s="3">
+      <c r="D2" s="16"/>
+      <c r="E2" s="3">
         <v>269</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>12435</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>210</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>1500</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>3405</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>5100</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="5">
         <v>540</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>930</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>540</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>100</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>227</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>62</v>
       </c>
-      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -14669,8 +14708,9 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
-    </row>
-    <row r="3" spans="1:35" s="15" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="1"/>
+    </row>
+    <row r="3" spans="1:36" s="15" customFormat="1" ht="11.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>17921</v>
       </c>
@@ -14678,43 +14718,45 @@
         <v>15</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
+        <v>17916</v>
+      </c>
+      <c r="E3" s="3">
         <v>65</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>2925</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>24</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>645</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>360</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <v>1020</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>450</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>210</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>450</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="5">
         <v>43</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="5">
         <v>24</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="5">
         <v>14</v>
       </c>
-      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -14734,8 +14776,9 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-    </row>
-    <row r="4" spans="1:35" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ3" s="1"/>
+    </row>
+    <row r="4" spans="1:36" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>17922</v>
       </c>
@@ -14743,43 +14786,45 @@
         <v>16</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
+        <v>17916</v>
+      </c>
+      <c r="E4" s="3">
         <v>63</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>2835</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>12</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>420</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>90</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>1290</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>315</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>630</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>315</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>28</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>6</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>42</v>
       </c>
-      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -14799,8 +14844,9 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
-    </row>
-    <row r="5" spans="1:35" s="15" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ4" s="1"/>
+    </row>
+    <row r="5" spans="1:36" s="15" customFormat="1" ht="11.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>17923</v>
       </c>
@@ -14808,43 +14854,45 @@
         <v>17</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
+        <v>17916</v>
+      </c>
+      <c r="E5" s="3">
         <v>85</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>3825</v>
       </c>
-      <c r="F5" s="5">
-        <v>30</v>
-      </c>
       <c r="G5" s="5">
+        <v>30</v>
+      </c>
+      <c r="H5" s="5">
         <v>510</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>240</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>1875</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>360</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>630</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>360</v>
       </c>
-      <c r="M5" s="5">
+      <c r="N5" s="5">
         <v>34</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>16</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <v>42</v>
       </c>
-      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -14864,6 +14912,7 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>